<commit_message>
still need to reformat tables
</commit_message>
<xml_diff>
--- a/paper/tables/Table2.xlsx
+++ b/paper/tables/Table2.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t xml:space="preserve">Variable</t>
   </si>
@@ -53,37 +53,37 @@
     <t xml:space="preserve">Amplification</t>
   </si>
   <si>
-    <t xml:space="preserve">Hearing Aid (53) / Cochlear Implant (17) / None (27)</t>
+    <t xml:space="preserve">Hearing Aid (53) / Cochlear Implant (17) / None (28)</t>
   </si>
   <si>
     <t xml:space="preserve">Communication</t>
   </si>
   <si>
-    <t xml:space="preserve">Spoken (78) / Total Communication (18) / Cued Speech (1)</t>
+    <t xml:space="preserve">Spoken (79) / Total Communication (18) / Cued Speech (1)</t>
   </si>
   <si>
     <t xml:space="preserve">Degree Hearing Loss (worse ear)</t>
   </si>
   <si>
-    <t xml:space="preserve">18-100 dB HL (mean (SD): 65 (23))</t>
+    <t xml:space="preserve">18-100 dB HL (mean (SD): 64 (23))</t>
   </si>
   <si>
     <t xml:space="preserve">Developmental Delay</t>
   </si>
   <si>
-    <t xml:space="preserve">Yes (16) / No (81)</t>
+    <t xml:space="preserve">Yes (16) / No (82)</t>
   </si>
   <si>
     <t xml:space="preserve">Gender</t>
   </si>
   <si>
-    <t xml:space="preserve">Female (44) / Male (56)</t>
+    <t xml:space="preserve">Female (43) / Male (57)</t>
   </si>
   <si>
     <t xml:space="preserve">Health Issues</t>
   </si>
   <si>
-    <t xml:space="preserve">Yes (35) / No (62)</t>
+    <t xml:space="preserve">Yes (36) / No (62)</t>
   </si>
   <si>
     <t xml:space="preserve">Language in Home</t>
@@ -95,37 +95,43 @@
     <t xml:space="preserve">Laterality</t>
   </si>
   <si>
-    <t xml:space="preserve">Unilateral (25) / Bilateral (72)</t>
+    <t xml:space="preserve">Unilateral (26) / Bilateral (72)</t>
   </si>
   <si>
     <t xml:space="preserve">1-3-6</t>
   </si>
   <si>
-    <t xml:space="preserve">Yes (35) / No (59)</t>
+    <t xml:space="preserve">Yes (34) / No (61)</t>
   </si>
   <si>
     <t xml:space="preserve">Premature Birth</t>
   </si>
   <si>
-    <t xml:space="preserve">Full-term (16) / Premature (81)</t>
+    <t xml:space="preserve">Full-term (16) / Premature (82)</t>
   </si>
   <si>
     <t xml:space="preserve">Services Per Month</t>
   </si>
   <si>
-    <t xml:space="preserve">0-43 services per month (mean (SD): 6 (6))</t>
+    <t xml:space="preserve">0-43 services per month (mean (SD): 5 (6))</t>
   </si>
   <si>
     <t xml:space="preserve">Etiology</t>
   </si>
   <si>
-    <t xml:space="preserve">Sensorineural (61) / Conductive (18) / Mixed (8)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CDI - Words Produced</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0-635 words (mean (SD): 61 (111))</t>
+    <t xml:space="preserve">Sensorineural (62) / Conductive (19) / Mixed (8)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Words and Gestures CDI - Words Produced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-259 words (mean (SD): 33 (53))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Words and Sentences CDI - Words Produced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7-635 words (mean (SD): 148 (184))</t>
   </si>
 </sst>
 </file>
@@ -609,6 +615,14 @@
         <v>37</v>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>